<commit_message>
update cost spreadsheets and figure label powerpoint
</commit_message>
<xml_diff>
--- a/2024_07_03_MEM_Costs.xlsx
+++ b/2024_07_03_MEM_Costs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annali/Documents/Third Storage Proofs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annali/Documents/MEM_public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16E6E61-18BC-0B4A-93A4-165D0094BD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AAF4D2-17C4-CD41-BBFB-9FA11C82C4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" xr2:uid="{9402D557-0539-F249-9981-FEF30EBBF85E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27900" windowHeight="17500" xr2:uid="{9402D557-0539-F249-9981-FEF30EBBF85E}"/>
   </bookViews>
   <sheets>
     <sheet name="Storage Techs" sheetId="8" r:id="rId1"/>
@@ -635,7 +635,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Metal-air batteries. The energy- and power-capacity costs provided are calculated using a total combined cost of 20 $/kWh and an assumed 100 h duration, as reported in Form Energy press releases. 4.95 $/kWh was attributed to energy-capacity and 1505 $/kW to power-capacity, based on the ratio of estimated 2020 energy-capacity cost (3.7 $/kWh) to 2020 mid power-capacity cost (1123.53 $/kW) provided in the 2022 MIT Future of Energy Storage report in Table 2.1. </t>
+      <t xml:space="preserve">Metal-air batteries. The energy- and power-capacity costs provided for metal-air batteires are calculated using a total overnight cost of 20 $/kWh and an assumed 100 h duration, as reported in Form Energy press releases. 4.95 $/kWh was attributed to energy-capacity and 1505 $/kW to power-capacity, based on the ratio of estimated 2020 energy-capacity cost (3.7 $/kWh) to 2020 mid power-capacity cost (1123.53 $/kW) provided in the 2022 MIT Future of Energy Storage report in Table 2.1. </t>
     </r>
     <r>
       <rPr>
@@ -646,7 +646,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>However, it should be noted that the final total fixed hourly cost calculated remains the same regardless of what costs are attributed to energy-capacity vs. power-capacity.</t>
+      <t xml:space="preserve">However, it should be noted that with a defined total overnight cost and duration, the total fixed hourly cost calculated remains the same regardless of what costs are attributed to energy-capacity vs. power-capacity. </t>
     </r>
     <r>
       <rPr>
@@ -656,7 +656,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> This is because 1) We already define that the total overnight cost is 20 $/kWh and that the duration is 100h, 2) the calculations for hourly fixed cost are linear operations on overnight fixed cost, and 3) the final fixed hourly cost is a total cost combining energy-capacity and power-capacity fixed hourly cost values.</t>
+      <t>This is because 1) the calculations for hourly fixed cost are linear operations on overnight fixed cost, and 2) the final fixed hourly cost is a total cost combining energy-capacity and power-capacity fixed hourly cost values. Remaining variables used to calculate the fixed hourly costs are taken from the MIT 2022 Future of Energy Storage report.</t>
     </r>
   </si>
 </sst>
@@ -1223,13 +1223,49 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1259,47 +1295,11 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2818,7 +2818,7 @@
   <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="J14" zoomScale="86" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+      <selection activeCell="U16" sqref="U16:V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2827,8 +2827,8 @@
     <col min="2" max="6" width="13.6640625" style="2" customWidth="1"/>
     <col min="7" max="15" width="14.6640625" style="2" customWidth="1"/>
     <col min="16" max="20" width="16" style="2" customWidth="1"/>
-    <col min="21" max="21" width="34.6640625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="35.33203125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="37.1640625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="38" style="2" customWidth="1"/>
     <col min="23" max="23" width="18" style="2" customWidth="1"/>
     <col min="24" max="27" width="17.5" style="2" customWidth="1"/>
     <col min="28" max="16384" width="10.83203125" style="2"/>
@@ -2843,29 +2843,29 @@
       <c r="A2" s="8"/>
     </row>
     <row r="3" spans="1:29" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
-      <c r="U3" s="67" t="s">
+      <c r="U3" s="79" t="s">
         <v>47</v>
       </c>
       <c r="V3" s="8"/>
@@ -2880,54 +2880,54 @@
       <c r="AC3" s="13"/>
     </row>
     <row r="4" spans="1:29" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67"/>
-      <c r="B4" s="68" t="s">
+      <c r="A4" s="79"/>
+      <c r="B4" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="68"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
       <c r="Q4" s="19"/>
       <c r="R4" s="19"/>
-      <c r="U4" s="67"/>
+      <c r="U4" s="79"/>
       <c r="V4" s="8"/>
       <c r="W4" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="67"/>
-      <c r="B5" s="68" t="s">
+      <c r="A5" s="79"/>
+      <c r="B5" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="68"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
       <c r="Q5" s="19"/>
       <c r="R5" s="19"/>
-      <c r="U5" s="67"/>
+      <c r="U5" s="79"/>
       <c r="V5" s="8"/>
       <c r="W5" s="13" t="s">
         <v>62</v>
@@ -2985,130 +2985,130 @@
     </row>
     <row r="13" spans="1:29" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
-      <c r="U13" s="66" t="s">
+      <c r="U13" s="71" t="s">
         <v>112</v>
       </c>
-      <c r="V13" s="66"/>
+      <c r="V13" s="71"/>
     </row>
     <row r="14" spans="1:29" ht="63.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="70"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="71"/>
-      <c r="O14" s="71"/>
-      <c r="P14" s="71"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="83"/>
+      <c r="L14" s="83"/>
+      <c r="M14" s="83"/>
+      <c r="N14" s="83"/>
+      <c r="O14" s="83"/>
+      <c r="P14" s="83"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
-      <c r="S14" s="66" t="s">
+      <c r="S14" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="T14" s="66"/>
-      <c r="U14" s="66" t="s">
+      <c r="T14" s="71"/>
+      <c r="U14" s="71" t="s">
         <v>113</v>
       </c>
-      <c r="V14" s="66"/>
+      <c r="V14" s="71"/>
     </row>
     <row r="15" spans="1:29" s="8" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="69" t="s">
+      <c r="C15" s="73"/>
+      <c r="D15" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="69"/>
-      <c r="F15" s="83" t="s">
+      <c r="E15" s="81"/>
+      <c r="F15" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="82" t="s">
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="73" t="s">
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="M15" s="73"/>
-      <c r="N15" s="75" t="s">
+      <c r="M15" s="85"/>
+      <c r="N15" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="O15" s="75"/>
-      <c r="P15" s="74" t="s">
+      <c r="O15" s="87"/>
+      <c r="P15" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74"/>
-      <c r="S15" s="76" t="s">
+      <c r="Q15" s="86"/>
+      <c r="R15" s="86"/>
+      <c r="S15" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="T15" s="76"/>
-      <c r="U15" s="81" t="s">
+      <c r="T15" s="72"/>
+      <c r="U15" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="V15" s="81"/>
+      <c r="V15" s="75"/>
     </row>
     <row r="16" spans="1:29" ht="182" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66" t="s">
+      <c r="C16" s="71"/>
+      <c r="D16" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66" t="s">
+      <c r="E16" s="71"/>
+      <c r="F16" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66" t="s">
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="J16" s="66"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66" t="s">
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66" t="s">
+      <c r="M16" s="71"/>
+      <c r="N16" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="O16" s="66"/>
-      <c r="P16" s="66" t="s">
+      <c r="O16" s="71"/>
+      <c r="P16" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="66"/>
-      <c r="S16" s="66" t="s">
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="T16" s="66"/>
-      <c r="U16" s="66" t="s">
+      <c r="T16" s="71"/>
+      <c r="U16" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="V16" s="66"/>
+      <c r="V16" s="71"/>
     </row>
     <row r="17" spans="1:27" s="8" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="40" t="s">
@@ -3255,10 +3255,10 @@
         <f>1430.07299270073*_2020_USD_to__2019_USD</f>
         <v>1415.9138541591387</v>
       </c>
-      <c r="U18" s="88">
+      <c r="U18" s="64">
         <v>4.9547046259499998</v>
       </c>
-      <c r="V18" s="89">
+      <c r="V18" s="65">
         <v>1504.5295374</v>
       </c>
     </row>
@@ -3757,11 +3757,11 @@
       <c r="A25" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="80">
+      <c r="B25" s="74">
         <f>B24+C24/4</f>
         <v>3.9573263954289966E-3</v>
       </c>
-      <c r="C25" s="80"/>
+      <c r="C25" s="74"/>
       <c r="D25" s="41"/>
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
@@ -3779,11 +3779,11 @@
       <c r="R25" s="41"/>
       <c r="S25" s="41"/>
       <c r="T25" s="41"/>
-      <c r="U25" s="64">
+      <c r="U25" s="77">
         <f>U24+V24/100</f>
         <v>2.143776335865519E-4</v>
       </c>
-      <c r="V25" s="65"/>
+      <c r="V25" s="78"/>
     </row>
     <row r="26" spans="1:27" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -4075,45 +4075,45 @@
       <c r="A30" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="77">
+      <c r="B30" s="66">
         <v>0.86</v>
       </c>
-      <c r="C30" s="78"/>
-      <c r="D30" s="77">
+      <c r="C30" s="67"/>
+      <c r="D30" s="66">
         <v>0.75</v>
       </c>
-      <c r="E30" s="78"/>
-      <c r="F30" s="77">
+      <c r="E30" s="67"/>
+      <c r="F30" s="66">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="77">
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="66">
         <v>0.65</v>
       </c>
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="77">
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="66">
         <v>0.81</v>
       </c>
-      <c r="M30" s="78"/>
-      <c r="N30" s="84">
+      <c r="M30" s="67"/>
+      <c r="N30" s="69">
         <v>0.52</v>
       </c>
-      <c r="O30" s="85"/>
-      <c r="P30" s="77">
+      <c r="O30" s="70"/>
+      <c r="P30" s="66">
         <v>0.36</v>
       </c>
-      <c r="Q30" s="78"/>
-      <c r="R30" s="78"/>
-      <c r="S30" s="77">
+      <c r="Q30" s="67"/>
+      <c r="R30" s="67"/>
+      <c r="S30" s="66">
         <v>0.84</v>
       </c>
-      <c r="T30" s="78"/>
-      <c r="U30" s="77">
+      <c r="T30" s="67"/>
+      <c r="U30" s="66">
         <v>0.46</v>
       </c>
-      <c r="V30" s="78"/>
+      <c r="V30" s="67"/>
     </row>
     <row r="31" spans="1:27" s="22" customFormat="1" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
@@ -4124,15 +4124,15 @@
     <row r="33" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="U3:U5"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="B14:P14"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:P4"/>
     <mergeCell ref="U30:V30"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B15:C15"/>
@@ -4147,17 +4147,17 @@
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="U25:V25"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="U3:U5"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="U14:V14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B14:P14"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="B4:P4"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
     <mergeCell ref="L15:M15"/>
     <mergeCell ref="P16:R16"/>
     <mergeCell ref="P15:R15"/>
@@ -4214,18 +4214,18 @@
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23"/>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="87"/>
-      <c r="D14" s="86" t="s">
+      <c r="C14" s="89"/>
+      <c r="D14" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="87"/>
-      <c r="F14" s="86" t="s">
+      <c r="E14" s="89"/>
+      <c r="F14" s="88" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="87"/>
+      <c r="G14" s="89"/>
     </row>
     <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
@@ -4585,12 +4585,12 @@
       <c r="B10" s="41">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">

</xml_diff>